<commit_message>
vault backup: 2025-10-19 14:54:04
</commit_message>
<xml_diff>
--- a/01 - Projets en Developpement/P002 - HLM/01 - Documentation de Projet/P002 - Documentation Conception.xlsx
+++ b/01 - Projets en Developpement/P002 - HLM/01 - Documentation de Projet/P002 - Documentation Conception.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\03 - Sonia Vault\01 - Projets en Developpement\P002 - HLM\01 - Documentation de Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD32FF2F-2FA4-4FCA-9A67-1BF2A438B06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A3B30-7E58-4F3C-B866-54A650C7B49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{82276768-738D-404D-9509-E52E01DFEC62}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82276768-738D-404D-9509-E52E01DFEC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="361">
   <si>
     <t>Overview</t>
   </si>
@@ -990,9 +990,6 @@
     <t>Le système doit être relativement compact.</t>
   </si>
   <si>
-    <t>Le système doit, dans la mesure du possible, utiliser des cartes de 10 × 10 cm pour éviter les surcoûts.</t>
-  </si>
-  <si>
     <t>Le système doit offrir la possibilité d’un accès extérieur pour déclencher une fonction de mission et/ou de kill.</t>
   </si>
   <si>
@@ -1005,9 +1002,6 @@
     <t>Le système doit pouvoir transmettre des informations visuelles sur son état (température, bugs, etc.).</t>
   </si>
   <si>
-    <t>Les systèmes, et plus précisément les cartes électroniques, doivent être clairs et faciles à utiliser (user-friendly).</t>
-  </si>
-  <si>
     <t>Le système doit avoir le moins possible de connecteurs différents (puissance, communication, etc.).</t>
   </si>
   <si>
@@ -1023,9 +1017,6 @@
     <t>Le système doit pouvoir alimenter l’ordinateur de bord.</t>
   </si>
   <si>
-    <t>Le système doit fournir différentes alimentations au reste du sous-marin (2 V, 12 V, etc.).</t>
-  </si>
-  <si>
     <t>Le système doit être résistant à l’électricité statique et disposer de protections (fusibles, diodes, etc.) en entrée et en sortie de fonction.</t>
   </si>
   <si>
@@ -1038,33 +1029,15 @@
     <t>Le système doit avoir une uniformisation de la BOM (liste de composants).</t>
   </si>
   <si>
-    <t>Le système doit utiliser des composants de taille standard 0603.</t>
-  </si>
-  <si>
     <t>Le système doit pouvoir supporter le fonctionnement d’une communication inter-sous-marins.</t>
   </si>
   <si>
-    <t>Les différentes parties du système doivent être isolées.</t>
-  </si>
-  <si>
-    <t>Le système doit pouvoir supporter la fonction hydrophone.</t>
-  </si>
-  <si>
     <t>Le système doit assumer la gestion d’un bras robotique avec un nombre variable d’axes.</t>
   </si>
   <si>
-    <t>Le système doit pouvoir fonctionner avec un seul pack batterie pour tout l’ordinateur.</t>
-  </si>
-  <si>
-    <t>Le système doit pouvoir couper toute alimentation des moteurs via un kill switch qui ne puisse pas être désactivé accidentellement.</t>
-  </si>
-  <si>
     <t>Le système doit pouvoir contrôler le sous-marin et toutes ses fonctions.</t>
   </si>
   <si>
-    <t>Chaque PCB du système doit être facilement testable via des points de test.</t>
-  </si>
-  <si>
     <t>Le système doit comporter le moins de microcontrôleurs possible.</t>
   </si>
   <si>
@@ -1074,9 +1047,6 @@
     <t>Le système doit avoir une autonomie minimale de 2 h pour un test régulier.</t>
   </si>
   <si>
-    <t>Le système doit pouvoir intégrer un BMS pour la protection des batteries.</t>
-  </si>
-  <si>
     <t>REQ1.5</t>
   </si>
   <si>
@@ -1125,9 +1095,6 @@
     <t>REQ1.20</t>
   </si>
   <si>
-    <t>Le système doit pouvoir être programmé via STM32Cube.</t>
-  </si>
-  <si>
     <t>Le système doit avoir une architecture avec un master et plusieurs slaves.</t>
   </si>
   <si>
@@ -1135,13 +1102,58 @@
   </si>
   <si>
     <t>REQ3.3</t>
+  </si>
+  <si>
+    <t>Le système doit fournir différentes alimentations au reste du sous-marin (5 V, 12 V, etc.).</t>
+  </si>
+  <si>
+    <t>Le système doit utiliser des composants de taille standard.</t>
+  </si>
+  <si>
+    <t>Les différentes parties du système doivent être isolées avec une approche modulaire.</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir supporter l'alimentation des hydrophones.</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir alimenter l'ordinateur et les fonctions critiques de securtié avec une seul batterie (interchangable).</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir couper toute alimentation des moteurs via un kill switch.</t>
+  </si>
+  <si>
+    <t>REQ1.21</t>
+  </si>
+  <si>
+    <t>Le systeme doit pouvoir alimenter et communiquer avec le DVL.</t>
+  </si>
+  <si>
+    <t>Chaque PCB du système doit être facilement testable via des points de test et documenté.</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir intégrer une communication avec le BMS pour la protection des batteries.</t>
+  </si>
+  <si>
+    <t>Les systèmes, et plus précisément les cartes électroniques, doivent être clairs et faciles à utiliser (user-friendly, connecteur identifié, detrompeur...).</t>
+  </si>
+  <si>
+    <t>Le système doit pouvoir être programmé avec un outils standard.</t>
+  </si>
+  <si>
+    <t>Le systeme doit permettre au mester de programmer les slaves</t>
+  </si>
+  <si>
+    <t>REQ3.4</t>
+  </si>
+  <si>
+    <t>Le système doit, dans la mesure du possible, utiliser des cartes de 10 × 10 cm ou moins pour éviter les surcoûts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1151,6 +1163,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1194,7 +1214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1552,11 +1572,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1692,15 +1723,18 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1716,9 +1750,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1746,6 +1777,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1756,12 +1793,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1795,6 +1826,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2171,15 +2207,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2189,14 +2225,14 @@
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -2206,56 +2242,56 @@
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>296</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="58"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="58"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
@@ -2273,7 +2309,7 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
+      <c r="A12" s="57"/>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2325,7 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -2299,12 +2335,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B7:G9"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2313,17 +2349,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1C7B82-BE6E-41CE-9DDC-946432E87E20}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="131.85546875" customWidth="1"/>
+    <col min="3" max="3" width="138.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,7 +2397,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,7 +2406,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2415,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,310 +2424,328 @@
         <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="70"/>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="70"/>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="70"/>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="70"/>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>324</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="70"/>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="70"/>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="70"/>
       <c r="B14" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="70"/>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="70"/>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="70"/>
       <c r="B17" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="70"/>
       <c r="B18" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="70"/>
       <c r="B19" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70"/>
-      <c r="B20" t="s">
-        <v>349</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>333</v>
+      <c r="B20" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="C20" s="93" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="70"/>
       <c r="B21" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="70"/>
       <c r="B22" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="71"/>
-      <c r="B23" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="70"/>
+      <c r="B23" t="s">
+        <v>342</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="71"/>
+      <c r="B24" t="s">
         <v>352</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="C24" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C25" s="94" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="67"/>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="67"/>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="67"/>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="67"/>
       <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="67"/>
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="68"/>
+      <c r="B30" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="69" t="s">
+      <c r="C30" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="69" t="s">
         <v>301</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C31" s="16" t="s">
         <v>302</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="70"/>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="70"/>
       <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="70"/>
+      <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="71"/>
-      <c r="B33" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>355</v>
+      <c r="C33" s="7" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="70"/>
+      <c r="B34" t="s">
+        <v>345</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="71"/>
+      <c r="B35" t="s">
+        <v>359</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C36" s="16" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" t="s">
-        <v>299</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" t="s">
-        <v>300</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="70"/>
       <c r="B37" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="70"/>
       <c r="B38" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="70"/>
+      <c r="B39" t="s">
+        <v>304</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="70"/>
+      <c r="B40" t="s">
+        <v>309</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="71"/>
+      <c r="B41" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="71"/>
-      <c r="B39" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="C39" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>307</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A3:A23"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A3:A24"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A36:A41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2728,11 +2782,11 @@
       <c r="B2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
       <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2743,8 +2797,8 @@
       <c r="C3" s="85">
         <v>45875</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2752,11 +2806,11 @@
       <c r="B4" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2780,14 +2834,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="79"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -3020,17 +3074,17 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="79"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="75" t="s">
         <v>126</v>
       </c>
       <c r="B21" t="s">
@@ -3118,7 +3172,7 @@
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
+      <c r="A26" s="76"/>
       <c r="B26" t="s">
         <v>167</v>
       </c>
@@ -3134,14 +3188,14 @@
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="80" t="s">
@@ -3252,17 +3306,17 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="77" t="s">
         <v>182</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="77"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="79"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="75" t="s">
         <v>201</v>
       </c>
       <c r="B35" t="s">
@@ -3428,17 +3482,17 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="77"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="79"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="78" t="s">
+      <c r="A45" s="75" t="s">
         <v>181</v>
       </c>
       <c r="B45" t="s">
@@ -3477,6 +3531,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A28:A33"/>
@@ -3488,11 +3547,6 @@
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3771,11 +3825,11 @@
       <c r="B2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
       <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3786,8 +3840,8 @@
       <c r="C3" s="85">
         <v>45875</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3795,11 +3849,11 @@
       <c r="B4" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3823,14 +3877,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="77" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="79"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -3869,14 +3923,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="79"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="80" t="s">
@@ -4075,17 +4129,17 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="77"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="79"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="75" t="s">
         <v>233</v>
       </c>
       <c r="B22" t="s">
@@ -4229,14 +4283,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="77" t="s">
         <v>249</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="77"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="79"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
@@ -4293,17 +4347,17 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="77" t="s">
         <v>255</v>
       </c>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="77"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="79"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="75" t="s">
         <v>255</v>
       </c>
       <c r="B35" t="s">
@@ -4357,7 +4411,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
+      <c r="A38" s="76"/>
       <c r="B38" t="s">
         <v>261</v>
       </c>
@@ -4375,17 +4429,17 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="77" t="s">
         <v>267</v>
       </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="77"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="79"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="78" t="s">
+      <c r="A40" s="75" t="s">
         <v>267</v>
       </c>
       <c r="B40" t="s">
@@ -4405,7 +4459,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="79"/>
+      <c r="A41" s="76"/>
       <c r="B41" t="s">
         <v>265</v>
       </c>
@@ -4423,14 +4477,14 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="77" t="s">
         <v>268</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="77"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="79"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="80" t="s">
@@ -4525,17 +4579,17 @@
       <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="75" t="s">
+      <c r="A48" s="77" t="s">
         <v>280</v>
       </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="77"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="78" t="s">
+      <c r="A49" s="75" t="s">
         <v>280</v>
       </c>
       <c r="B49" t="s">
@@ -4690,11 +4744,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:A57"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:A20"/>
     <mergeCell ref="A39:F39"/>
@@ -4706,10 +4759,11 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4998,11 +5052,11 @@
       <c r="C2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="38" t="s">
         <v>60</v>
       </c>
@@ -5011,16 +5065,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -5260,16 +5314,16 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="79"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -5573,14 +5627,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>